<commit_message>
Operações matemáticas e ajustes de texto
</commit_message>
<xml_diff>
--- a/C#/json_to_xlsx/Example.xlsx
+++ b/C#/json_to_xlsx/Example.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Dados" sheetId="1" r:id="rId1"/>
+    <sheet name="Movies" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -26,7 +26,7 @@
     <t>genre</t>
   </si>
   <si>
-    <t>Back to the Future</t>
+    <t>De volta para o futuro</t>
   </si>
   <si>
     <t>1985</t>
@@ -35,10 +35,10 @@
     <t>Marty McFly</t>
   </si>
   <si>
-    <t>Science fiction</t>
+    <t>Ficção Científica</t>
   </si>
   <si>
-    <t>Ferris Bueller's Day Off</t>
+    <t>Vivendo a vida adoidado</t>
   </si>
   <si>
     <t>1986</t>
@@ -47,7 +47,7 @@
     <t>Matthew Broderick</t>
   </si>
   <si>
-    <t>Comedy</t>
+    <t>Comédia</t>
   </si>
 </sst>
 </file>

</xml_diff>